<commit_message>
add information to data
</commit_message>
<xml_diff>
--- a/full_data/overall_sub&obj_risk.xlsx
+++ b/full_data/overall_sub&obj_risk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\研究生任务资料\研一任务\6. 主客观数据处理\6. 开源数据处理\开源材料示例\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\吴新政个人文件夹\研究生各学习任务\研4\2024.10.23数据开源小论文ITSC\开源网站\RISEE_dataset\full_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DA679C-3DA8-44BD-B95C-995ED6CDA752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBEB17A-F1F4-43A2-8E14-78381EBB0428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7150" yWindow="340" windowWidth="17460" windowHeight="14090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-7250" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="各场景客观风险指标计算结果" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sub_risk</t>
+    <t>SUB_avg</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A180"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>